<commit_message>
change children with between 4-15
</commit_message>
<xml_diff>
--- a/data/UNICEF_Data.xlsx
+++ b/data/UNICEF_Data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25412"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25423"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://polymtlca0-my.sharepoint.com/personal/georg-aaron_seitfudem_polymtl_ca/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3898B8EC-15E6-42E3-9625-522B62C51246}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5924323E-1E27-4A23-B60D-B0A5966C1841}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -769,7 +769,7 @@
     <t>stillbirth</t>
   </si>
   <si>
-    <t>children</t>
+    <t>between 5-14</t>
   </si>
   <si>
     <t>Iran (Islamic Republic of)</t>
@@ -25223,10 +25223,13 @@
   <dimension ref="A1:F995"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="6" max="6" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="25" t="s">

</xml_diff>